<commit_message>
removed code duplication, added link to sample plan in readme
</commit_message>
<xml_diff>
--- a/tests/data/test.xlsx
+++ b/tests/data/test.xlsx
@@ -1589,7 +1589,7 @@
         <v>67</v>
       </c>
       <c r="B22" s="2">
-        <f>'A1'!P8</f>
+        <f>'A1'!P1</f>
         <v>0</v>
       </c>
       <c r="C22" s="2">
@@ -1606,7 +1606,7 @@
         <v>68</v>
       </c>
       <c r="B23" s="2">
-        <f>'B2U4'!P6</f>
+        <f>'B2U4'!P1</f>
         <v>0</v>
       </c>
       <c r="C23" s="2">
@@ -2368,7 +2368,7 @@
         <v>67</v>
       </c>
       <c r="B20" s="2">
-        <f>'A1'!Q8</f>
+        <f>'A1'!Q1</f>
         <v>0</v>
       </c>
       <c r="C20" s="2">
@@ -2385,7 +2385,7 @@
         <v>68</v>
       </c>
       <c r="B21" s="2">
-        <f>'B2U4'!Q6</f>
+        <f>'B2U4'!Q1</f>
         <v>0</v>
       </c>
       <c r="C21" s="2">
@@ -3128,7 +3128,7 @@
         <v>79</v>
       </c>
       <c r="B24" s="2">
-        <f>'A1'!S8</f>
+        <f>'A1'!S1</f>
         <v>0</v>
       </c>
       <c r="C24" s="2">
@@ -3230,7 +3230,7 @@
         <v>80</v>
       </c>
       <c r="B30" s="2">
-        <f>'B2U4'!S6</f>
+        <f>'B2U4'!S1</f>
         <v>0</v>
       </c>
       <c r="C30" s="2">
@@ -3973,7 +3973,7 @@
         <v>79</v>
       </c>
       <c r="B24" s="2">
-        <f>'A1'!T8</f>
+        <f>'A1'!T1</f>
         <v>0</v>
       </c>
       <c r="C24" s="2">
@@ -4075,7 +4075,7 @@
         <v>80</v>
       </c>
       <c r="B30" s="2">
-        <f>'B2U4'!T6</f>
+        <f>'B2U4'!T1</f>
         <v>0</v>
       </c>
       <c r="C30" s="2">

</xml_diff>